<commit_message>
Update UI Login for APP
</commit_message>
<xml_diff>
--- a/Haircut Management/WorkFlowTime.xlsx
+++ b/Haircut Management/WorkFlowTime.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Link :</t>
   </si>
@@ -157,6 +157,22 @@
         <scheme val="minor"/>
       </rPr>
       <t>https://www.youtube.com/watch?v=Hc9qK9xJjiU&amp;t=1121s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Icon : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://www.freepik.com/icon/cancel_18249285#fromView=search&amp;page=1&amp;position=53&amp;uuid=f2f2c95e-2154-4e04-85b1-eb58e78ed2be</t>
     </r>
   </si>
 </sst>
@@ -541,10 +557,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -596,6 +612,11 @@
         <v>13</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Complete UI convert views for button slide bar
</commit_message>
<xml_diff>
--- a/Haircut Management/WorkFlowTime.xlsx
+++ b/Haircut Management/WorkFlowTime.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Link :</t>
   </si>
@@ -173,6 +173,38 @@
         <scheme val="minor"/>
       </rPr>
       <t>https://www.freepik.com/icon/cancel_18249285#fromView=search&amp;page=1&amp;position=53&amp;uuid=f2f2c95e-2154-4e04-85b1-eb58e78ed2be</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>sub menu silder bar:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> https://youtu.be/E5NB9crfQZs?si=Q8c77KPhtsqENjsh </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>main :</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> https://www.youtube.com/watch?v=CkHyDYeImjY</t>
     </r>
   </si>
 </sst>
@@ -557,10 +589,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,6 +649,16 @@
         <v>14</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>